<commit_message>
fix: fixed demand category bug
- fixed demand category reading and writing
- added test for demand category reading and writing
- added demand categories to Junction J-02 in Poulakis_enhanced_PDA.inp and updated results file
</commit_message>
<xml_diff>
--- a/testing/networks/Poulakis_enhanced_PDA.xlsx
+++ b/testing/networks/Poulakis_enhanced_PDA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\tiuri\PycharmProjects\oopnet\testing\networks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\oopnet\testing\networks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1148D5B-A419-4491-8CA7-77C0D68C8D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046FE050-F968-4623-97AE-B3FDF6F293FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6C77D1FC-2AC6-4423-9F71-9CA578A46760}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8928" activeTab="1" xr2:uid="{6C77D1FC-2AC6-4423-9F71-9CA578A46760}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -391,8 +391,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -709,13 +710,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B298A4-EFC1-4A4A-9B24-C9172563D442}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="N27" sqref="J1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -732,7 +733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -740,16 +741,16 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="D2">
-        <v>47.97</v>
+        <v>47.87</v>
       </c>
       <c r="E2">
-        <v>47.97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47.87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -760,13 +761,13 @@
         <v>50</v>
       </c>
       <c r="D3">
-        <v>34.659999999999997</v>
+        <v>34.56</v>
       </c>
       <c r="E3">
-        <v>34.659999999999997</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34.56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -777,13 +778,13 @@
         <v>50</v>
       </c>
       <c r="D4">
-        <v>32.65</v>
+        <v>32.549999999999997</v>
       </c>
       <c r="E4">
-        <v>32.65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32.549999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>78</v>
       </c>
@@ -794,13 +795,13 @@
         <v>50</v>
       </c>
       <c r="D5">
-        <v>25.48</v>
+        <v>25.39</v>
       </c>
       <c r="E5">
-        <v>25.48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25.39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>79</v>
       </c>
@@ -811,13 +812,13 @@
         <v>50</v>
       </c>
       <c r="D6">
-        <v>23.73</v>
+        <v>23.63</v>
       </c>
       <c r="E6">
-        <v>23.73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23.63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -825,16 +826,16 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>69.87</v>
+        <v>69.78</v>
       </c>
       <c r="D7">
-        <v>19.87</v>
+        <v>19.78</v>
       </c>
       <c r="E7">
-        <v>19.87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19.78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -845,13 +846,13 @@
         <v>50</v>
       </c>
       <c r="D8">
-        <v>35.200000000000003</v>
+        <v>35.1</v>
       </c>
       <c r="E8">
-        <v>35.200000000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -862,13 +863,13 @@
         <v>50</v>
       </c>
       <c r="D9">
-        <v>34.25</v>
+        <v>34.15</v>
       </c>
       <c r="E9">
-        <v>34.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -879,13 +880,13 @@
         <v>50</v>
       </c>
       <c r="D10">
-        <v>32.71</v>
+        <v>32.61</v>
       </c>
       <c r="E10">
-        <v>32.71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32.61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>84</v>
       </c>
@@ -896,13 +897,13 @@
         <v>50</v>
       </c>
       <c r="D11">
-        <v>24.4</v>
+        <v>24.31</v>
       </c>
       <c r="E11">
-        <v>24.4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24.31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>85</v>
       </c>
@@ -913,13 +914,13 @@
         <v>50</v>
       </c>
       <c r="D12">
-        <v>23.07</v>
+        <v>22.98</v>
       </c>
       <c r="E12">
-        <v>23.07</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22.98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>86</v>
       </c>
@@ -930,13 +931,13 @@
         <v>50</v>
       </c>
       <c r="D13">
-        <v>19.82</v>
+        <v>19.73</v>
       </c>
       <c r="E13">
-        <v>19.82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19.73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -947,13 +948,13 @@
         <v>50</v>
       </c>
       <c r="D14">
-        <v>31.41</v>
+        <v>31.31</v>
       </c>
       <c r="E14">
-        <v>31.41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31.31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>88</v>
       </c>
@@ -964,13 +965,13 @@
         <v>50</v>
       </c>
       <c r="D15">
-        <v>30.89</v>
+        <v>30.79</v>
       </c>
       <c r="E15">
-        <v>30.89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30.79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>89</v>
       </c>
@@ -981,13 +982,13 @@
         <v>50</v>
       </c>
       <c r="D16">
-        <v>29.8</v>
+        <v>29.7</v>
       </c>
       <c r="E16">
-        <v>29.8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>90</v>
       </c>
@@ -998,13 +999,13 @@
         <v>50</v>
       </c>
       <c r="D17">
-        <v>23.7</v>
+        <v>23.61</v>
       </c>
       <c r="E17">
-        <v>23.7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23.61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>91</v>
       </c>
@@ -1015,13 +1016,13 @@
         <v>50</v>
       </c>
       <c r="D18">
-        <v>24.4</v>
+        <v>24.31</v>
       </c>
       <c r="E18">
-        <v>24.4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24.31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>92</v>
       </c>
@@ -1032,13 +1033,13 @@
         <v>50</v>
       </c>
       <c r="D19">
-        <v>18.98</v>
+        <v>18.89</v>
       </c>
       <c r="E19">
-        <v>18.98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18.89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>93</v>
       </c>
@@ -1049,13 +1050,13 @@
         <v>50</v>
       </c>
       <c r="D20">
-        <v>25.23</v>
+        <v>25.13</v>
       </c>
       <c r="E20">
-        <v>25.23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25.13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>94</v>
       </c>
@@ -1066,13 +1067,13 @@
         <v>50</v>
       </c>
       <c r="D21">
-        <v>24.67</v>
+        <v>24.57</v>
       </c>
       <c r="E21">
-        <v>24.67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24.57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -1083,13 +1084,13 @@
         <v>50</v>
       </c>
       <c r="D22">
-        <v>15.89</v>
+        <v>15.79</v>
       </c>
       <c r="E22">
-        <v>15.89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15.79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>96</v>
       </c>
@@ -1100,13 +1101,13 @@
         <v>50</v>
       </c>
       <c r="D23">
-        <v>15.48</v>
+        <v>15.39</v>
       </c>
       <c r="E23">
-        <v>15.48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15.39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>97</v>
       </c>
@@ -1117,13 +1118,13 @@
         <v>50</v>
       </c>
       <c r="D24">
-        <v>14.43</v>
+        <v>14.34</v>
       </c>
       <c r="E24">
-        <v>14.43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14.34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>98</v>
       </c>
@@ -1134,145 +1135,145 @@
         <v>50</v>
       </c>
       <c r="D25">
-        <v>13.45</v>
+        <v>13.37</v>
       </c>
       <c r="E25">
-        <v>13.45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13.37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>99</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>50</v>
       </c>
-      <c r="D26">
-        <v>22.94</v>
-      </c>
-      <c r="E26">
-        <v>22.94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="1">
+        <v>22.84</v>
+      </c>
+      <c r="E26" s="1">
+        <v>22.84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>100</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>50</v>
       </c>
-      <c r="D27">
-        <v>19.829999999999998</v>
-      </c>
-      <c r="E27">
-        <v>19.829999999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D27" s="1">
+        <v>19.739999999999998</v>
+      </c>
+      <c r="E27" s="1">
+        <v>19.739999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>101</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>50</v>
       </c>
-      <c r="D28">
-        <v>15.86</v>
-      </c>
-      <c r="E28">
-        <v>15.86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D28" s="1">
+        <v>15.77</v>
+      </c>
+      <c r="E28" s="1">
+        <v>15.77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>102</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>50</v>
       </c>
-      <c r="D29">
-        <v>15.22</v>
-      </c>
-      <c r="E29">
-        <v>15.22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="1">
+        <v>15.13</v>
+      </c>
+      <c r="E29" s="1">
+        <v>15.13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>103</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
-      <c r="C30">
-        <v>49.8</v>
-      </c>
-      <c r="D30">
-        <v>9.92</v>
-      </c>
-      <c r="E30">
-        <v>9.92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="1">
+        <v>49.62</v>
+      </c>
+      <c r="D30" s="1">
+        <v>9.85</v>
+      </c>
+      <c r="E30" s="1">
+        <v>9.85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>104</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
-      <c r="C31">
-        <v>49.8</v>
-      </c>
-      <c r="D31">
-        <v>9.92</v>
-      </c>
-      <c r="E31">
-        <v>9.92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C31" s="1">
+        <v>49.62</v>
+      </c>
+      <c r="D31" s="1">
+        <v>9.85</v>
+      </c>
+      <c r="E31" s="1">
+        <v>9.85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>105</v>
       </c>
       <c r="B32">
         <v>52</v>
       </c>
-      <c r="C32">
-        <v>-1519.48</v>
-      </c>
-      <c r="D32">
+      <c r="C32" s="1">
+        <v>-1540.03</v>
+      </c>
+      <c r="D32" s="1">
         <v>52</v>
       </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>106</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33">
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
         <v>10</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="1">
         <v>10</v>
       </c>
     </row>
@@ -1283,44 +1284,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E732489E-0A09-48F1-B339-75EEE610C8CC}">
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="8" width="11.44140625" style="1"/>
+    <col min="11" max="24" width="11.44140625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1330,26 +1335,26 @@
       <c r="C2">
         <v>600</v>
       </c>
-      <c r="D2">
-        <v>1519.48</v>
-      </c>
-      <c r="E2">
-        <v>5.37</v>
-      </c>
-      <c r="F2">
-        <v>40.26</v>
-      </c>
-      <c r="G2">
+      <c r="D2" s="1">
+        <v>1540.03</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5.45</v>
+      </c>
+      <c r="F2" s="1">
+        <v>41.35</v>
+      </c>
+      <c r="G2" s="1">
         <v>1.6E-2</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <v>0</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1359,26 +1364,26 @@
       <c r="C3">
         <v>600</v>
       </c>
-      <c r="D3">
-        <v>869.75</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="1">
+        <v>869.49</v>
+      </c>
+      <c r="E3" s="1">
         <v>3.08</v>
       </c>
-      <c r="F3">
-        <v>13.31</v>
-      </c>
-      <c r="G3">
+      <c r="F3" s="1">
+        <v>13.3</v>
+      </c>
+      <c r="G3" s="1">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>0</v>
       </c>
       <c r="I3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1388,26 +1393,26 @@
       <c r="C4">
         <v>600</v>
       </c>
-      <c r="D4">
-        <v>332.86</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="1">
+        <v>332.77</v>
+      </c>
+      <c r="E4" s="1">
         <v>1.18</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>2.0099999999999998</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1">
         <v>0</v>
       </c>
       <c r="I4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1417,26 +1422,26 @@
       <c r="C5">
         <v>450</v>
       </c>
-      <c r="D5">
-        <v>299.17</v>
-      </c>
-      <c r="E5">
+      <c r="D5" s="1">
+        <v>299.08</v>
+      </c>
+      <c r="E5" s="1">
         <v>1.88</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>7.17</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1">
         <v>0</v>
       </c>
       <c r="I5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1446,26 +1451,26 @@
       <c r="C6">
         <v>450</v>
       </c>
-      <c r="D6">
-        <v>145.87</v>
-      </c>
-      <c r="E6">
+      <c r="D6" s="1">
+        <v>145.82</v>
+      </c>
+      <c r="E6" s="1">
         <v>0.92</v>
       </c>
-      <c r="F6">
-        <v>1.76</v>
-      </c>
-      <c r="G6">
+      <c r="F6" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="G6" s="1">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1">
         <v>0</v>
       </c>
       <c r="I6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1475,26 +1480,26 @@
       <c r="C7">
         <v>300</v>
       </c>
-      <c r="D7">
-        <v>75.02</v>
-      </c>
-      <c r="E7">
+      <c r="D7" s="1">
+        <v>74.97</v>
+      </c>
+      <c r="E7" s="1">
         <v>1.06</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>3.85</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>0.02</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="1">
         <v>0</v>
       </c>
       <c r="I7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1504,26 +1509,26 @@
       <c r="C8">
         <v>600</v>
       </c>
-      <c r="D8">
-        <v>599.73</v>
-      </c>
-      <c r="E8">
+      <c r="D8" s="1">
+        <v>599.54</v>
+      </c>
+      <c r="E8" s="1">
         <v>2.12</v>
       </c>
-      <c r="F8">
-        <v>6.39</v>
-      </c>
-      <c r="G8">
+      <c r="F8" s="1">
+        <v>6.38</v>
+      </c>
+      <c r="G8" s="1">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="1">
         <v>0</v>
       </c>
       <c r="I8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1533,26 +1538,26 @@
       <c r="C9">
         <v>600</v>
       </c>
-      <c r="D9">
-        <v>102.38</v>
-      </c>
-      <c r="E9">
+      <c r="D9" s="1">
+        <v>102.32</v>
+      </c>
+      <c r="E9" s="1">
         <v>0.36</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>0.21</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="1">
         <v>0</v>
       </c>
       <c r="I9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1562,26 +1567,26 @@
       <c r="C10">
         <v>450</v>
       </c>
-      <c r="D10">
-        <v>-16.309999999999999</v>
-      </c>
-      <c r="E10">
+      <c r="D10" s="1">
+        <v>-16.32</v>
+      </c>
+      <c r="E10" s="1">
         <v>0.1</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>0.03</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>2.3E-2</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="1">
         <v>0</v>
       </c>
       <c r="I10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1591,26 +1596,26 @@
       <c r="C11">
         <v>450</v>
       </c>
-      <c r="D11">
-        <v>79.19</v>
-      </c>
-      <c r="E11">
+      <c r="D11" s="1">
+        <v>79.17</v>
+      </c>
+      <c r="E11" s="1">
         <v>0.5</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>0.54</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>1.9E-2</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="1">
         <v>0</v>
       </c>
       <c r="I11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1620,26 +1625,26 @@
       <c r="C12">
         <v>300</v>
       </c>
-      <c r="D12">
-        <v>20.85</v>
-      </c>
-      <c r="E12">
+      <c r="D12" s="1">
+        <v>20.84</v>
+      </c>
+      <c r="E12" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>0.33</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="1">
         <v>0</v>
       </c>
       <c r="I12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1649,26 +1654,26 @@
       <c r="C13">
         <v>300</v>
       </c>
-      <c r="D13">
-        <v>5.15</v>
-      </c>
-      <c r="E13">
+      <c r="D13" s="1">
+        <v>5.19</v>
+      </c>
+      <c r="E13" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F13">
-        <v>0.02</v>
-      </c>
-      <c r="G13">
+      <c r="F13" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="G13" s="1">
         <v>2.7E-2</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="1">
         <v>0</v>
       </c>
       <c r="I13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1678,26 +1683,26 @@
       <c r="C14">
         <v>600</v>
       </c>
-      <c r="D14">
-        <v>226.73</v>
-      </c>
-      <c r="E14">
+      <c r="D14" s="1">
+        <v>226.67</v>
+      </c>
+      <c r="E14" s="1">
         <v>0.8</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>0.95</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="1">
         <v>0</v>
       </c>
       <c r="I14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1707,26 +1712,26 @@
       <c r="C15">
         <v>450</v>
       </c>
-      <c r="D15">
-        <v>136.46</v>
-      </c>
-      <c r="E15">
+      <c r="D15" s="1">
+        <v>136.43</v>
+      </c>
+      <c r="E15" s="1">
         <v>0.86</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>1.54</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
         <v>1.9E-2</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="1">
         <v>0</v>
       </c>
       <c r="I15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1736,26 +1741,26 @@
       <c r="C16">
         <v>450</v>
       </c>
-      <c r="D16">
-        <v>322.27999999999997</v>
-      </c>
-      <c r="E16">
+      <c r="D16" s="1">
+        <v>322.2</v>
+      </c>
+      <c r="E16" s="1">
         <v>2.0299999999999998</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1">
         <v>8.3000000000000007</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="1">
         <v>0</v>
       </c>
       <c r="I16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1765,26 +1770,26 @@
       <c r="C17">
         <v>300</v>
       </c>
-      <c r="D17">
-        <v>43.46</v>
-      </c>
-      <c r="E17">
+      <c r="D17" s="1">
+        <v>43.44</v>
+      </c>
+      <c r="E17" s="1">
         <v>0.61</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <v>1.33</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="1">
         <v>0</v>
       </c>
       <c r="I17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1794,26 +1799,26 @@
       <c r="C18">
         <v>300</v>
       </c>
-      <c r="D18">
-        <v>68.709999999999994</v>
-      </c>
-      <c r="E18">
+      <c r="D18" s="1">
+        <v>68.67</v>
+      </c>
+      <c r="E18" s="1">
         <v>0.97</v>
       </c>
-      <c r="F18">
-        <v>3.25</v>
-      </c>
-      <c r="G18">
+      <c r="F18" s="1">
+        <v>3.24</v>
+      </c>
+      <c r="G18" s="1">
         <v>0.02</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="1">
         <v>0</v>
       </c>
       <c r="I18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1823,26 +1828,26 @@
       <c r="C19">
         <v>600</v>
       </c>
-      <c r="D19">
-        <v>323</v>
-      </c>
-      <c r="E19">
+      <c r="D19" s="1">
+        <v>322.87</v>
+      </c>
+      <c r="E19" s="1">
         <v>1.1399999999999999</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <v>1.89</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="1">
         <v>0</v>
       </c>
       <c r="I19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1852,26 +1857,26 @@
       <c r="C20">
         <v>450</v>
       </c>
-      <c r="D20">
-        <v>142.65</v>
-      </c>
-      <c r="E20">
+      <c r="D20" s="1">
+        <v>142.56</v>
+      </c>
+      <c r="E20" s="1">
         <v>0.9</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <v>1.68</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="1">
         <v>0</v>
       </c>
       <c r="I20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1881,26 +1886,26 @@
       <c r="C21">
         <v>450</v>
       </c>
-      <c r="D21">
-        <v>132.38</v>
-      </c>
-      <c r="E21">
+      <c r="D21" s="1">
+        <v>132.32</v>
+      </c>
+      <c r="E21" s="1">
         <v>0.83</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <v>1.45</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="1">
         <v>1.9E-2</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="1">
         <v>0</v>
       </c>
       <c r="I21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -1910,26 +1915,26 @@
       <c r="C22">
         <v>300</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>21.6</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="1">
         <v>0.31</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="1">
         <v>0.35</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="1">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="1">
         <v>0</v>
       </c>
       <c r="I22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1939,26 +1944,26 @@
       <c r="C23">
         <v>300</v>
       </c>
-      <c r="D23">
-        <v>-30.29</v>
-      </c>
-      <c r="E23">
+      <c r="D23" s="1">
+        <v>-30.28</v>
+      </c>
+      <c r="E23" s="1">
         <v>0.43</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="1">
         <v>0.67</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="1">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="1">
         <v>0</v>
       </c>
       <c r="I23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -1968,26 +1973,26 @@
       <c r="C24">
         <v>300</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>23.86</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="1">
         <v>0.34</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="1">
         <v>0.42</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="1">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="1">
         <v>0</v>
       </c>
       <c r="I24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -1997,26 +2002,26 @@
       <c r="C25">
         <v>450</v>
       </c>
-      <c r="D25">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="E25">
+      <c r="D25" s="1">
+        <v>77.989999999999995</v>
+      </c>
+      <c r="E25" s="1">
         <v>0.49</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="1">
         <v>0.52</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="1">
         <v>1.9E-2</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="1">
         <v>0</v>
       </c>
       <c r="I25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -2026,26 +2031,26 @@
       <c r="C26">
         <v>450</v>
       </c>
-      <c r="D26">
-        <v>113.99</v>
-      </c>
-      <c r="E26">
+      <c r="D26" s="1">
+        <v>114.03</v>
+      </c>
+      <c r="E26" s="1">
         <v>0.72</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="1">
         <v>1.0900000000000001</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="1">
         <v>1.9E-2</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="1">
         <v>0</v>
       </c>
       <c r="I26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -2055,26 +2060,26 @@
       <c r="C27">
         <v>300</v>
       </c>
-      <c r="D27">
-        <v>94.88</v>
-      </c>
-      <c r="E27">
+      <c r="D27" s="1">
+        <v>94.87</v>
+      </c>
+      <c r="E27" s="1">
         <v>1.34</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="1">
         <v>6.1</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="1">
         <v>0.02</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="1">
         <v>0</v>
       </c>
       <c r="I27" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -2084,26 +2089,26 @@
       <c r="C28">
         <v>300</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>-31.09</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <v>0.44</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="1">
         <v>0.7</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="1">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="1">
         <v>0</v>
       </c>
       <c r="I28" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -2113,26 +2118,26 @@
       <c r="C29">
         <v>300</v>
       </c>
-      <c r="D29">
-        <v>89.4</v>
-      </c>
-      <c r="E29">
+      <c r="D29" s="1">
+        <v>89.36</v>
+      </c>
+      <c r="E29" s="1">
         <v>1.26</v>
       </c>
-      <c r="F29">
-        <v>5.43</v>
-      </c>
-      <c r="G29">
+      <c r="F29" s="1">
+        <v>5.42</v>
+      </c>
+      <c r="G29" s="1">
         <v>0.02</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="1">
         <v>0</v>
       </c>
       <c r="I29" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -2142,26 +2147,26 @@
       <c r="C30">
         <v>450</v>
       </c>
-      <c r="D30">
-        <v>194.9</v>
-      </c>
-      <c r="E30">
+      <c r="D30" s="1">
+        <v>194.88</v>
+      </c>
+      <c r="E30" s="1">
         <v>1.23</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="1">
         <v>3.09</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="1">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="1">
         <v>0</v>
       </c>
       <c r="I30" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -2171,26 +2176,26 @@
       <c r="C31">
         <v>450</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>195.54</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="1">
         <v>1.23</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="1">
         <v>3.11</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="1">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="1">
         <v>0</v>
       </c>
       <c r="I31" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -2200,26 +2205,26 @@
       <c r="C32">
         <v>300</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <v>101.48</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="1">
         <v>1.44</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="1">
         <v>6.96</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="1">
         <v>0.02</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="1">
         <v>0</v>
       </c>
       <c r="I32" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -2229,26 +2234,26 @@
       <c r="C33">
         <v>300</v>
       </c>
-      <c r="D33">
-        <v>77.58</v>
-      </c>
-      <c r="E33">
+      <c r="D33" s="1">
+        <v>77.56</v>
+      </c>
+      <c r="E33" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="1">
         <v>4.1100000000000003</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="1">
         <v>0.02</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="1">
         <v>0</v>
       </c>
       <c r="I33" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -2258,26 +2263,26 @@
       <c r="C34">
         <v>300</v>
       </c>
-      <c r="D34">
-        <v>85.63</v>
-      </c>
-      <c r="E34">
+      <c r="D34" s="1">
+        <v>85.59</v>
+      </c>
+      <c r="E34" s="1">
         <v>1.21</v>
       </c>
-      <c r="F34">
-        <v>4.99</v>
-      </c>
-      <c r="G34">
+      <c r="F34" s="1">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="G34" s="1">
         <v>0.02</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="1">
         <v>0</v>
       </c>
       <c r="I34" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -2287,26 +2292,26 @@
       <c r="C35">
         <v>300</v>
       </c>
-      <c r="D35">
-        <v>63.26</v>
-      </c>
-      <c r="E35">
+      <c r="D35" s="1">
+        <v>63.22</v>
+      </c>
+      <c r="E35" s="1">
         <v>0.89</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="1">
         <v>2.76</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="1">
         <v>0.02</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="1">
         <v>0</v>
       </c>
       <c r="I35" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>51</v>
       </c>
@@ -2316,26 +2321,26 @@
       <c r="C36">
         <v>300</v>
       </c>
-      <c r="D36">
-        <v>27.75</v>
-      </c>
-      <c r="E36">
+      <c r="D36" s="1">
+        <v>27.74</v>
+      </c>
+      <c r="E36" s="1">
         <v>0.39</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="1">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="1">
         <v>0</v>
       </c>
       <c r="I36" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -2345,26 +2350,26 @@
       <c r="C37">
         <v>300</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>114.24</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="1">
         <v>1.62</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="1">
         <v>8.7799999999999994</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="1">
         <v>0.02</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="1">
         <v>0</v>
       </c>
       <c r="I37" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>53</v>
       </c>
@@ -2374,26 +2379,26 @@
       <c r="C38">
         <v>300</v>
       </c>
-      <c r="D38">
-        <v>23.44</v>
-      </c>
-      <c r="E38">
+      <c r="D38" s="1">
+        <v>23.3</v>
+      </c>
+      <c r="E38" s="1">
         <v>0.33</v>
       </c>
-      <c r="F38">
-        <v>0.41</v>
-      </c>
-      <c r="G38">
+      <c r="F38" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="G38" s="1">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="1">
         <v>0</v>
       </c>
       <c r="I38" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -2403,26 +2408,26 @@
       <c r="C39">
         <v>300</v>
       </c>
-      <c r="D39">
-        <v>38.33</v>
-      </c>
-      <c r="E39">
+      <c r="D39" s="1">
+        <v>38.22</v>
+      </c>
+      <c r="E39" s="1">
         <v>0.54</v>
       </c>
-      <c r="F39">
-        <v>1.05</v>
-      </c>
-      <c r="G39">
+      <c r="F39" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="G39" s="1">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="1">
         <v>0</v>
       </c>
       <c r="I39" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -2432,26 +2437,26 @@
       <c r="C40">
         <v>300</v>
       </c>
-      <c r="D40">
-        <v>36.97</v>
-      </c>
-      <c r="E40">
+      <c r="D40" s="1">
+        <v>36.92</v>
+      </c>
+      <c r="E40" s="1">
         <v>0.52</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="1">
         <v>0.98</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="1">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="1">
         <v>0</v>
       </c>
       <c r="I40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>56</v>
       </c>
@@ -2461,26 +2466,26 @@
       <c r="C41">
         <v>450</v>
       </c>
-      <c r="D41">
-        <v>117.15</v>
-      </c>
-      <c r="E41">
+      <c r="D41" s="1">
+        <v>117.14</v>
+      </c>
+      <c r="E41" s="1">
         <v>0.74</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="1">
         <v>1.1499999999999999</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="1">
         <v>1.9E-2</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="1">
         <v>0</v>
       </c>
       <c r="I41" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>57</v>
       </c>
@@ -2490,26 +2495,26 @@
       <c r="C42">
         <v>300</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
         <v>59.04</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="1">
         <v>0.84</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="1">
         <v>2.42</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="1">
         <v>0.02</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="1">
         <v>0</v>
       </c>
       <c r="I42" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -2519,26 +2524,26 @@
       <c r="C43">
         <v>300</v>
       </c>
-      <c r="D43">
-        <v>3.51</v>
-      </c>
-      <c r="E43">
+      <c r="D43" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="E43" s="1">
         <v>0.05</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="1">
         <v>0.01</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="1">
         <v>0.03</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="1">
         <v>0</v>
       </c>
       <c r="I43" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>59</v>
       </c>
@@ -2548,26 +2553,26 @@
       <c r="C44">
         <v>300</v>
       </c>
-      <c r="D44">
-        <v>12.68</v>
-      </c>
-      <c r="E44">
+      <c r="D44" s="1">
+        <v>12.64</v>
+      </c>
+      <c r="E44" s="1">
         <v>0.18</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="1">
         <v>0.13</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="1">
         <v>2.4E-2</v>
       </c>
-      <c r="H44">
+      <c r="H44" s="1">
         <v>0</v>
       </c>
       <c r="I44" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>60</v>
       </c>
@@ -2577,26 +2582,26 @@
       <c r="C45">
         <v>300</v>
       </c>
-      <c r="D45">
-        <v>56.98</v>
-      </c>
-      <c r="E45">
-        <v>0.81</v>
-      </c>
-      <c r="F45">
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="G45">
+      <c r="D45" s="1">
+        <v>56.89</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F45" s="1">
+        <v>2.25</v>
+      </c>
+      <c r="G45" s="1">
         <v>0.02</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="1">
         <v>0</v>
       </c>
       <c r="I45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>61</v>
       </c>
@@ -2606,26 +2611,26 @@
       <c r="C46">
         <v>300</v>
       </c>
-      <c r="D46">
-        <v>50.23</v>
-      </c>
-      <c r="E46">
+      <c r="D46" s="1">
+        <v>50.14</v>
+      </c>
+      <c r="E46" s="1">
         <v>0.71</v>
       </c>
-      <c r="F46">
-        <v>1.77</v>
-      </c>
-      <c r="G46">
+      <c r="F46" s="1">
+        <v>1.76</v>
+      </c>
+      <c r="G46" s="1">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="H46">
+      <c r="H46" s="1">
         <v>0</v>
       </c>
       <c r="I46" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>62</v>
       </c>
@@ -2635,26 +2640,26 @@
       <c r="C47">
         <v>300</v>
       </c>
-      <c r="D47">
-        <v>67.150000000000006</v>
-      </c>
-      <c r="E47">
+      <c r="D47" s="1">
+        <v>67.14</v>
+      </c>
+      <c r="E47" s="1">
         <v>0.95</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="1">
         <v>3.1</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="1">
         <v>0.02</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="1">
         <v>0</v>
       </c>
       <c r="I47" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -2664,26 +2669,26 @@
       <c r="C48">
         <v>300</v>
       </c>
-      <c r="D48">
-        <v>76.19</v>
-      </c>
-      <c r="E48">
+      <c r="D48" s="1">
+        <v>76.180000000000007</v>
+      </c>
+      <c r="E48" s="1">
         <v>1.08</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="1">
         <v>3.97</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="1">
         <v>0.02</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="1">
         <v>0</v>
       </c>
       <c r="I48" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>64</v>
       </c>
@@ -2693,26 +2698,26 @@
       <c r="C49">
         <v>300</v>
       </c>
-      <c r="D49">
-        <v>29.7</v>
-      </c>
-      <c r="E49">
+      <c r="D49" s="1">
+        <v>29.58</v>
+      </c>
+      <c r="E49" s="1">
         <v>0.42</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="1">
         <v>0.64</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="1">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="1">
         <v>0</v>
       </c>
       <c r="I49" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>65</v>
       </c>
@@ -2722,26 +2727,26 @@
       <c r="C50">
         <v>300</v>
       </c>
-      <c r="D50">
-        <v>88.33</v>
-      </c>
-      <c r="E50">
+      <c r="D50" s="1">
+        <v>88.17</v>
+      </c>
+      <c r="E50" s="1">
         <v>1.25</v>
       </c>
-      <c r="F50">
-        <v>5.3</v>
-      </c>
-      <c r="G50">
+      <c r="F50" s="1">
+        <v>5.28</v>
+      </c>
+      <c r="G50" s="1">
         <v>0.02</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="1">
         <v>0</v>
       </c>
       <c r="I50" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>66</v>
       </c>
@@ -2751,26 +2756,26 @@
       <c r="C51">
         <v>300</v>
       </c>
-      <c r="D51">
-        <v>-0.43</v>
-      </c>
-      <c r="E51">
+      <c r="D51" s="1">
+        <v>-0.52</v>
+      </c>
+      <c r="E51" s="1">
         <v>0.01</v>
       </c>
-      <c r="F51">
-        <v>0</v>
-      </c>
-      <c r="G51">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="H51">
+      <c r="F51" s="1">
+        <v>0</v>
+      </c>
+      <c r="G51" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="H51" s="1">
         <v>0</v>
       </c>
       <c r="I51" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>67</v>
       </c>
@@ -2780,222 +2785,222 @@
       <c r="C52">
         <v>600</v>
       </c>
-      <c r="D52">
-        <v>0</v>
-      </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-      <c r="F52">
-        <v>0</v>
-      </c>
-      <c r="G52">
-        <v>0</v>
-      </c>
-      <c r="H52">
+      <c r="D52" s="1">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0</v>
+      </c>
+      <c r="H52" s="1">
         <v>0</v>
       </c>
       <c r="I52" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>74</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D53">
-        <v>95.94</v>
-      </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
-      <c r="F53">
-        <v>-5.3</v>
-      </c>
-      <c r="G53">
-        <v>0</v>
-      </c>
-      <c r="H53">
+      <c r="D53" s="1">
+        <v>95.96</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <v>-5.28</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0</v>
+      </c>
+      <c r="H53" s="1">
         <v>0</v>
       </c>
       <c r="I53" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>68</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C54">
         <v>500</v>
       </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
-      </c>
-      <c r="F54">
-        <v>0</v>
-      </c>
-      <c r="G54">
-        <v>0</v>
-      </c>
-      <c r="H54">
+      <c r="D54" s="1">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <v>0</v>
+      </c>
+      <c r="G54" s="1">
+        <v>0</v>
+      </c>
+      <c r="H54" s="1">
         <v>0</v>
       </c>
       <c r="I54" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>69</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C55">
         <v>500</v>
       </c>
-      <c r="D55">
-        <v>286.41000000000003</v>
-      </c>
-      <c r="E55">
+      <c r="D55" s="1">
+        <v>286.32</v>
+      </c>
+      <c r="E55" s="1">
         <v>1.46</v>
       </c>
-      <c r="F55">
-        <v>0</v>
-      </c>
-      <c r="G55">
-        <v>0</v>
-      </c>
-      <c r="H55">
+      <c r="F55" s="1">
+        <v>0</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0</v>
+      </c>
+      <c r="H55" s="1">
         <v>0</v>
       </c>
       <c r="I55" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>70</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C56">
         <v>500</v>
       </c>
-      <c r="D56">
-        <v>-138.78</v>
-      </c>
-      <c r="E56">
+      <c r="D56" s="1">
+        <v>-139.03</v>
+      </c>
+      <c r="E56" s="1">
         <v>0.71</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="1">
         <v>15</v>
       </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-      <c r="H56">
+      <c r="G56" s="1">
+        <v>0</v>
+      </c>
+      <c r="H56" s="1">
         <v>0</v>
       </c>
       <c r="I56" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>71</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C57">
         <v>500</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="1">
         <v>20</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="1">
         <v>0.1</v>
       </c>
-      <c r="F57">
-        <v>9.27</v>
-      </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-      <c r="H57">
+      <c r="F57" s="1">
+        <v>9.26</v>
+      </c>
+      <c r="G57" s="1">
+        <v>0</v>
+      </c>
+      <c r="H57" s="1">
         <v>0</v>
       </c>
       <c r="I57" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>72</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C58">
         <v>500</v>
       </c>
-      <c r="D58">
-        <v>384.51</v>
-      </c>
-      <c r="E58">
+      <c r="D58" s="1">
+        <v>384.4</v>
+      </c>
+      <c r="E58" s="1">
         <v>1.96</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="1">
         <v>1.95</v>
       </c>
-      <c r="G58">
-        <v>0</v>
-      </c>
-      <c r="H58">
+      <c r="G58" s="1">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1">
         <v>0</v>
       </c>
       <c r="I58" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>73</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C59">
         <v>500</v>
       </c>
-      <c r="D59">
-        <v>24.12</v>
-      </c>
-      <c r="E59">
+      <c r="D59" s="1">
+        <v>24.1</v>
+      </c>
+      <c r="E59" s="1">
         <v>0.12</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="1">
         <v>2.41</v>
       </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-      <c r="H59">
+      <c r="G59" s="1">
+        <v>0</v>
+      </c>
+      <c r="H59" s="1">
         <v>0</v>
       </c>
       <c r="I59" t="s">

</xml_diff>